<commit_message>
make everything better, relative path ok now
</commit_message>
<xml_diff>
--- a/Underwater_Robot_NFC/bin/Debug/underwater_robot_balance.xlsx
+++ b/Underwater_Robot_NFC/bin/Debug/underwater_robot_balance.xlsx
@@ -118,6 +118,926 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$1:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>No.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>No.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>No.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>No.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>No.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>No.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>No.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>No.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>No.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>No.10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>No.11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>No.12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>No.13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>No.14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>495</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3D4E-4DF0-B73F-08FCD054424B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1309313120"/>
+        <c:axId val="1303869728"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1309313120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1303869728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1303869728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1309313120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AD1C9AC-D2B6-496F-8B54-CFC7C5C6E49B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -420,7 +1340,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,7 +1350,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>470</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -438,7 +1358,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>500</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -446,7 +1366,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>500</v>
+        <v>495</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -454,7 +1374,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>500</v>
+        <v>480</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -462,7 +1382,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>500</v>
+        <v>410</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -502,7 +1422,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -510,7 +1430,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>500</v>
+        <v>460</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -518,7 +1438,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>500</v>
+        <v>455</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -526,7 +1446,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>500</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -539,5 +1459,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add ten btn bug fixed
</commit_message>
<xml_diff>
--- a/Underwater_Robot_NFC/bin/Debug/underwater_robot_balance.xlsx
+++ b/Underwater_Robot_NFC/bin/Debug/underwater_robot_balance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\robotics_team\underwater_nfc\Underwater_Robot_NFC\Underwater_Robot_NFC\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\robotics_team\underwater_nfc\Underwater_Robot_NFC\Underwater_Robot_NFC\bin\Release\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>No.1</t>
   </si>
@@ -66,6 +66,18 @@
   </si>
   <si>
     <t>No.14</t>
+  </si>
+  <si>
+    <t>No.15</t>
+  </si>
+  <si>
+    <t>No.16</t>
+  </si>
+  <si>
+    <t>No.17</t>
+  </si>
+  <si>
+    <t>No.18</t>
   </si>
 </sst>
 </file>
@@ -135,6 +147,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-HK"/>
+              <a:t>Team Balance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -186,9 +223,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$1:$A$14</c:f>
+              <c:f>Sheet1!$A$1:$A$18</c:f>
               <c:strCache>
-                <c:ptCount val="14"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>No.1</c:v>
                 </c:pt>
@@ -230,33 +267,45 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>No.14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>No.15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>No.16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>No.17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>No.18</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$14</c:f>
+              <c:f>Sheet1!$B$1:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>390</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>340</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>495</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>275</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>410</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>250</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>500</c:v>
@@ -268,18 +317,30 @@
                   <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>455</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>244</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>500</c:v>
                 </c:pt>
               </c:numCache>
@@ -300,7 +361,6 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
         <c:axId val="1309313120"/>
         <c:axId val="1303869728"/>
       </c:barChart>
@@ -1003,16 +1063,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1337,10 +1397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1350,7 +1410,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>390</v>
+        <v>500</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1358,7 +1418,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>340</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1366,7 +1426,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>495</v>
+        <v>500</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1374,7 +1434,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>275</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1382,7 +1442,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>410</v>
+        <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1390,7 +1450,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>250</v>
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1422,7 +1482,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1430,7 +1490,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -1438,7 +1498,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>455</v>
+        <v>500</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -1446,7 +1506,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>244</v>
+        <v>500</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -1454,6 +1514,38 @@
         <v>13</v>
       </c>
       <c r="B14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
         <v>500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added comfirmation screen upon trade request, allowed excel updates to show in real time
</commit_message>
<xml_diff>
--- a/Underwater_Robot_NFC/bin/Debug/underwater_robot_balance.xlsx
+++ b/Underwater_Robot_NFC/bin/Debug/underwater_robot_balance.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\robotics_team\underwater_nfc\Underwater_Robot_NFC\Underwater_Robot_NFC\bin\Release\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcreng\git\Underwater_Robot_NFC\Underwater_Robot_NFC\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -305,7 +305,7 @@
                   <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>500</c:v>
+                  <c:v>428</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>500</c:v>
@@ -1396,11 +1396,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1450,7 +1450,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>500</v>
+        <v>428</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Using new NFC.xlsx as Excel host, with transaction log and pivot table now
</commit_message>
<xml_diff>
--- a/Underwater_Robot_NFC/bin/Debug/underwater_robot_balance.xlsx
+++ b/Underwater_Robot_NFC/bin/Debug/underwater_robot_balance.xlsx
@@ -305,7 +305,7 @@
                   <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>428</c:v>
+                  <c:v>397</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>500</c:v>
@@ -1450,7 +1450,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>428</v>
+        <v>397</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>